<commit_message>
added premiums data as pbi example to read data from excel
</commit_message>
<xml_diff>
--- a/CPS_MDCR_PREMIUMS_2021.xlsx
+++ b/CPS_MDCR_PREMIUMS_2021.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bpkin\Downloads\CPS MDCR PREMIUMS 2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bpkin\OneDrive\Documents\PowerBI\datasets-power-bi-training\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8FA3D26-38A6-44E7-AFA6-062731F93D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE4335A-3A7D-4E74-AC15-EF0BC85FFD46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table of Contents" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,25 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="6">'MDCR PREMIUMS 6'!$3:$3,'MDCR PREMIUMS 6'!$A:$A</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="146">
   <si>
     <t>Medicare Premiums</t>
   </si>
@@ -229,163 +242,10 @@
     <t>United States</t>
   </si>
   <si>
-    <t>Alabama</t>
-  </si>
-  <si>
-    <t>Alaska</t>
-  </si>
-  <si>
-    <t>Arizona</t>
-  </si>
-  <si>
-    <t>Arkansas</t>
-  </si>
-  <si>
-    <t>California</t>
-  </si>
-  <si>
-    <t>Colorado</t>
-  </si>
-  <si>
-    <t>Connecticut</t>
-  </si>
-  <si>
-    <t>Delaware</t>
-  </si>
-  <si>
-    <t>District of Columbia</t>
-  </si>
-  <si>
-    <t>Florida</t>
-  </si>
-  <si>
-    <t>Georgia</t>
-  </si>
-  <si>
-    <t>Hawaii</t>
-  </si>
-  <si>
-    <t>Idaho</t>
-  </si>
-  <si>
-    <t>Illinois</t>
-  </si>
-  <si>
-    <t>Indiana</t>
-  </si>
-  <si>
-    <t>Iowa</t>
-  </si>
-  <si>
-    <t>Kansas</t>
-  </si>
-  <si>
-    <t>Kentucky</t>
-  </si>
-  <si>
-    <t>Louisiana</t>
-  </si>
-  <si>
-    <t>Maine</t>
-  </si>
-  <si>
-    <t>Maryland</t>
-  </si>
-  <si>
-    <t>Massachusetts</t>
-  </si>
-  <si>
-    <t>Michigan</t>
-  </si>
-  <si>
-    <t>Minnesota</t>
-  </si>
-  <si>
-    <t>Mississippi</t>
-  </si>
-  <si>
-    <t>Missouri</t>
-  </si>
-  <si>
     <t>Montana</t>
   </si>
   <si>
-    <t>Nebraska</t>
-  </si>
-  <si>
-    <t>Nevada</t>
-  </si>
-  <si>
-    <t>New Hampshire</t>
-  </si>
-  <si>
-    <t>New Jersey</t>
-  </si>
-  <si>
-    <t>New Mexico</t>
-  </si>
-  <si>
-    <t>New York</t>
-  </si>
-  <si>
-    <t>North Carolina</t>
-  </si>
-  <si>
-    <t>North Dakota</t>
-  </si>
-  <si>
-    <t>Ohio</t>
-  </si>
-  <si>
-    <t>Oklahoma</t>
-  </si>
-  <si>
-    <t>Oregon</t>
-  </si>
-  <si>
-    <t>Pennsylvania</t>
-  </si>
-  <si>
-    <t>Rhode Island</t>
-  </si>
-  <si>
-    <t>South Carolina</t>
-  </si>
-  <si>
-    <t>South Dakota</t>
-  </si>
-  <si>
-    <t>Tennessee</t>
-  </si>
-  <si>
-    <t>Texas</t>
-  </si>
-  <si>
-    <t>Utah</t>
-  </si>
-  <si>
-    <t>Vermont</t>
-  </si>
-  <si>
-    <t>Virginia</t>
-  </si>
-  <si>
-    <t>Washington</t>
-  </si>
-  <si>
-    <t>West Virginia</t>
-  </si>
-  <si>
-    <t>Wisconsin</t>
-  </si>
-  <si>
-    <t>Wyoming</t>
-  </si>
-  <si>
     <t>Territories, Possessions, and Other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Puerto Rico</t>
   </si>
   <si>
     <t xml:space="preserve">  U.S. Territories²</t>
@@ -1486,7 +1346,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="78" t="s">
-        <v>143</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
@@ -1510,7 +1370,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="78" t="s">
-        <v>144</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="33.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
@@ -2878,11 +2738,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I74"/>
+  <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2898,7 +2758,7 @@
     <col min="9" max="9" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2911,7 +2771,7 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>62</v>
       </c>
@@ -2924,7 +2784,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="55.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="55.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>63</v>
       </c>
@@ -2953,13 +2813,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>29</v>
       </c>
       <c r="I4" s="48"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>64</v>
       </c>
@@ -2988,7 +2848,7 @@
         <v>16646051</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>65</v>
       </c>
@@ -3017,7 +2877,7 @@
         <v>16632943</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>29</v>
       </c>
@@ -3030,9 +2890,9 @@
       <c r="H7" s="14"/>
       <c r="I7" s="10"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>145</v>
+        <v>94</v>
       </c>
       <c r="B8" s="10">
         <v>2563</v>
@@ -3058,10 +2918,14 @@
       <c r="I8" s="12">
         <v>149950</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J8">
+        <f>H8/B8</f>
+        <v>0.11158798283261803</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>146</v>
+        <v>95</v>
       </c>
       <c r="B9" s="10">
         <v>634</v>
@@ -3087,10 +2951,14 @@
       <c r="I9" s="15">
         <v>5888</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J9" t="e">
+        <f t="shared" ref="J9:J64" si="0">H9/B9</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>147</v>
+        <v>96</v>
       </c>
       <c r="B10" s="10">
         <v>4344</v>
@@ -3116,10 +2984,14 @@
       <c r="I10" s="15">
         <v>305369</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>0.13029465930018416</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>148</v>
+        <v>97</v>
       </c>
       <c r="B11" s="10">
         <v>2162</v>
@@ -3145,10 +3017,14 @@
       <c r="I11" s="15">
         <v>9693</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>8.7881591119333951E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>149</v>
+        <v>98</v>
       </c>
       <c r="B12" s="10">
         <v>181135</v>
@@ -3174,10 +3050,14 @@
       <c r="I12" s="15">
         <v>8524326</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>8.5952466392469701E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>150</v>
+        <v>99</v>
       </c>
       <c r="B13" s="10">
         <v>1118</v>
@@ -3203,10 +3083,14 @@
       <c r="I13" s="15">
         <v>68232</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>0.11806797853309481</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>151</v>
+        <v>100</v>
       </c>
       <c r="B14" s="10">
         <v>2759</v>
@@ -3232,10 +3116,14 @@
       <c r="I14" s="15">
         <v>82115</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>5.6904675607104022E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>152</v>
+        <v>101</v>
       </c>
       <c r="B15" s="10">
         <v>770</v>
@@ -3261,10 +3149,14 @@
       <c r="I15" s="15">
         <v>7348</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>1.6883116883116882E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>153</v>
+        <v>102</v>
       </c>
       <c r="B16" s="10">
         <v>2474</v>
@@ -3290,10 +3182,14 @@
       <c r="I16" s="15">
         <v>23055</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>1.6976556184316895E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>154</v>
+        <v>103</v>
       </c>
       <c r="B17" s="10">
         <v>108883</v>
@@ -3319,10 +3215,14 @@
       <c r="I17" s="15">
         <v>615997</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>1.0552611518786221E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
-        <v>155</v>
+        <v>104</v>
       </c>
       <c r="B18" s="10">
         <v>2660</v>
@@ -3348,10 +3248,14 @@
       <c r="I18" s="15">
         <v>104589</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>7.4436090225563911E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>156</v>
+        <v>105</v>
       </c>
       <c r="B19" s="10">
         <v>3674</v>
@@ -3377,10 +3281,14 @@
       <c r="I19" s="15">
         <v>27904</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>1.4153511159499184E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
-        <v>157</v>
+        <v>106</v>
       </c>
       <c r="B20" s="10">
         <v>549</v>
@@ -3406,10 +3314,14 @@
       <c r="I20" s="15">
         <v>11278</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>3.825136612021858E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>158</v>
+        <v>107</v>
       </c>
       <c r="B21" s="10">
         <v>5129</v>
@@ -3435,10 +3347,14 @@
       <c r="I21" s="15">
         <v>200538</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>7.5063365178397345E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>159</v>
+        <v>108</v>
       </c>
       <c r="B22" s="10">
         <v>1785</v>
@@ -3464,10 +3380,14 @@
       <c r="I22" s="15">
         <v>26941</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>2.8011204481792718E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
-        <v>160</v>
+        <v>109</v>
       </c>
       <c r="B23" s="10">
         <v>3106</v>
@@ -3493,10 +3413,14 @@
       <c r="I23" s="15">
         <v>16711</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>9.9806825499034121E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>161</v>
+        <v>110</v>
       </c>
       <c r="B24" s="10">
         <v>748</v>
@@ -3522,10 +3446,14 @@
       <c r="I24" s="15">
         <v>28184</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>6.9518716577540107E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>162</v>
+        <v>111</v>
       </c>
       <c r="B25" s="10">
         <v>1060</v>
@@ -3551,10 +3479,14 @@
       <c r="I25" s="15">
         <v>19687</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J25">
+        <f t="shared" si="0"/>
+        <v>3.6792452830188678E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>163</v>
+        <v>112</v>
       </c>
       <c r="B26" s="10">
         <v>9987</v>
@@ -3580,10 +3512,14 @@
       <c r="I26" s="15">
         <v>29039</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>5.507159307099229E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>164</v>
+        <v>113</v>
       </c>
       <c r="B27" s="10">
         <v>333</v>
@@ -3609,10 +3545,14 @@
       <c r="I27" s="15">
         <v>14440</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J27">
+        <f t="shared" si="0"/>
+        <v>9.3093093093093091E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
-        <v>165</v>
+        <v>114</v>
       </c>
       <c r="B28" s="10">
         <v>16933</v>
@@ -3638,10 +3578,14 @@
       <c r="I28" s="15">
         <v>114884</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J28">
+        <f t="shared" si="0"/>
+        <v>1.2165593810901789E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
-        <v>166</v>
+        <v>115</v>
       </c>
       <c r="B29" s="10">
         <v>34370</v>
@@ -3667,10 +3611,14 @@
       <c r="I29" s="15">
         <v>412142</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J29">
+        <f t="shared" si="0"/>
+        <v>2.3159732324701775E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
-        <v>167</v>
+        <v>116</v>
       </c>
       <c r="B30" s="10">
         <v>27997</v>
@@ -3696,10 +3644,14 @@
       <c r="I30" s="15">
         <v>57976</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J30">
+        <f t="shared" si="0"/>
+        <v>4.0361467300067868E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
-        <v>168</v>
+        <v>117</v>
       </c>
       <c r="B31" s="10">
         <v>10172</v>
@@ -3725,10 +3677,14 @@
       <c r="I31" s="15">
         <v>36186</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J31">
+        <f t="shared" si="0"/>
+        <v>6.685017695635077E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
-        <v>169</v>
+        <v>118</v>
       </c>
       <c r="B32" s="10">
         <v>5885</v>
@@ -3754,10 +3710,14 @@
       <c r="I32" s="15">
         <v>9401</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J32">
+        <f t="shared" si="0"/>
+        <v>2.8887000849617673E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
-        <v>170</v>
+        <v>119</v>
       </c>
       <c r="B33" s="10">
         <v>1958</v>
@@ -3783,10 +3743,14 @@
       <c r="I33" s="15">
         <v>77658</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J33">
+        <f t="shared" si="0"/>
+        <v>7.3544433094994893E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
-        <v>171</v>
+        <v>120</v>
       </c>
       <c r="B34" s="10">
         <v>831</v>
@@ -3812,10 +3776,14 @@
       <c r="I34" s="15">
         <v>4371</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J34" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="s">
-        <v>172</v>
+        <v>121</v>
       </c>
       <c r="B35" s="10">
         <v>132</v>
@@ -3841,10 +3809,14 @@
       <c r="I35" s="15">
         <v>6622</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J35">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090912E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
-        <v>173</v>
+        <v>122</v>
       </c>
       <c r="B36" s="10">
         <v>6747</v>
@@ -3870,10 +3842,14 @@
       <c r="I36" s="15">
         <v>56128</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J36">
+        <f t="shared" si="0"/>
+        <v>1.6007114273010228E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
-        <v>174</v>
+        <v>123</v>
       </c>
       <c r="B37" s="10">
         <v>264</v>
@@ -3899,10 +3875,14 @@
       <c r="I37" s="15">
         <v>19539</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J37">
+        <f t="shared" si="0"/>
+        <v>0.14015151515151514</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
-        <v>175</v>
+        <v>124</v>
       </c>
       <c r="B38" s="10">
         <v>18702</v>
@@ -3928,10 +3908,14 @@
       <c r="I38" s="15">
         <v>2583158</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J38">
+        <f t="shared" si="0"/>
+        <v>0.25253983531173135</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
-        <v>176</v>
+        <v>125</v>
       </c>
       <c r="B39" s="10">
         <v>612</v>
@@ -3957,10 +3941,14 @@
       <c r="I39" s="15">
         <v>39834</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J39">
+        <f t="shared" si="0"/>
+        <v>0.12091503267973856</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
-        <v>177</v>
+        <v>126</v>
       </c>
       <c r="B40" s="10">
         <v>136749</v>
@@ -3986,10 +3974,14 @@
       <c r="I40" s="15">
         <v>267918</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J40">
+        <f t="shared" si="0"/>
+        <v>3.6270831962208132E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
-        <v>178</v>
+        <v>127</v>
       </c>
       <c r="B41" s="10">
         <v>7876</v>
@@ -4015,10 +4007,14 @@
       <c r="I41" s="15">
         <v>71398</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J41">
+        <f t="shared" si="0"/>
+        <v>1.6886744540375826E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
-        <v>179</v>
+        <v>128</v>
       </c>
       <c r="B42" s="10">
         <v>111</v>
@@ -4044,10 +4040,14 @@
       <c r="I42" s="15">
         <v>2444</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J42" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
-        <v>180</v>
+        <v>129</v>
       </c>
       <c r="B43" s="10">
         <v>15104</v>
@@ -4073,10 +4073,14 @@
       <c r="I43" s="15">
         <v>1322694</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J43">
+        <f t="shared" si="0"/>
+        <v>0.171875</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
-        <v>181</v>
+        <v>130</v>
       </c>
       <c r="B44" s="10">
         <v>2628</v>
@@ -4102,10 +4106,14 @@
       <c r="I44" s="15">
         <v>23079</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J44">
+        <f t="shared" si="0"/>
+        <v>1.5601217656012176E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
-        <v>182</v>
+        <v>131</v>
       </c>
       <c r="B45" s="10">
         <v>8198</v>
@@ -4131,10 +4139,14 @@
       <c r="I45" s="15">
         <v>42669</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J45">
+        <f t="shared" si="0"/>
+        <v>1.000243961941937E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
-        <v>183</v>
+        <v>132</v>
       </c>
       <c r="B46" s="10">
         <v>25944</v>
@@ -4160,10 +4172,14 @@
       <c r="I46" s="15">
         <v>116270</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J46">
+        <f t="shared" si="0"/>
+        <v>8.3641689793401176E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
-        <v>184</v>
+        <v>133</v>
       </c>
       <c r="B47" s="10">
         <v>1479</v>
@@ -4189,10 +4205,14 @@
       <c r="I47" s="15">
         <v>11285</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J47">
+        <f t="shared" si="0"/>
+        <v>1.555104800540906E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
-        <v>185</v>
+        <v>134</v>
       </c>
       <c r="B48" s="10">
         <v>2198</v>
@@ -4218,10 +4238,14 @@
       <c r="I48" s="15">
         <v>46291</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J48">
+        <f t="shared" si="0"/>
+        <v>4.0946314831665151E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="9" t="s">
-        <v>186</v>
+        <v>135</v>
       </c>
       <c r="B49" s="10">
         <v>1541</v>
@@ -4247,10 +4271,14 @@
       <c r="I49" s="15">
         <v>2854</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J49" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
-        <v>187</v>
+        <v>136</v>
       </c>
       <c r="B50" s="10">
         <v>7566</v>
@@ -4276,10 +4304,14 @@
       <c r="I50" s="15">
         <v>42446</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J50">
+        <f t="shared" si="0"/>
+        <v>1.0573618821041502E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="9" t="s">
-        <v>188</v>
+        <v>137</v>
       </c>
       <c r="B51" s="10">
         <v>57586</v>
@@ -4305,10 +4337,14 @@
       <c r="I51" s="15">
         <v>351375</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J51">
+        <f t="shared" si="0"/>
+        <v>1.1495849685687494E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="s">
-        <v>189</v>
+        <v>138</v>
       </c>
       <c r="B52" s="10">
         <v>254</v>
@@ -4334,10 +4370,14 @@
       <c r="I52" s="15">
         <v>13706</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J52">
+        <f t="shared" si="0"/>
+        <v>0.1062992125984252</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="9" t="s">
-        <v>190</v>
+        <v>139</v>
       </c>
       <c r="B53" s="10">
         <v>892</v>
@@ -4363,10 +4403,14 @@
       <c r="I53" s="15">
         <v>2185</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J53" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="9" t="s">
-        <v>191</v>
+        <v>140</v>
       </c>
       <c r="B54" s="10">
         <v>6315</v>
@@ -4392,10 +4436,14 @@
       <c r="I54" s="15">
         <v>453358</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J54">
+        <f t="shared" si="0"/>
+        <v>0.13095803642121931</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="9" t="s">
-        <v>192</v>
+        <v>141</v>
       </c>
       <c r="B55" s="10">
         <v>25850</v>
@@ -4421,10 +4469,14 @@
       <c r="I55" s="15">
         <v>139520</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J55">
+        <f t="shared" si="0"/>
+        <v>1.0019342359767891E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="9" t="s">
-        <v>193</v>
+        <v>142</v>
       </c>
       <c r="B56" s="10">
         <v>4795</v>
@@ -4450,10 +4502,14 @@
       <c r="I56" s="15">
         <v>10743</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J56">
+        <f t="shared" si="0"/>
+        <v>4.3795620437956208E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="9" t="s">
-        <v>194</v>
+        <v>143</v>
       </c>
       <c r="B57" s="10">
         <v>7294</v>
@@ -4479,10 +4535,14 @@
       <c r="I57" s="15">
         <v>22959</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J57">
+        <f t="shared" si="0"/>
+        <v>5.8952563751028244E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="9" t="s">
-        <v>195</v>
+        <v>144</v>
       </c>
       <c r="B58" s="10">
         <v>182</v>
@@ -4508,22 +4568,34 @@
       <c r="I58" s="15">
         <v>565</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J58" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="16" t="s">
         <v>29</v>
       </c>
       <c r="I59" s="56"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J59" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="17" t="s">
-        <v>117</v>
+        <v>67</v>
       </c>
       <c r="I60" s="57"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J60" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="9" t="s">
-        <v>196</v>
+        <v>145</v>
       </c>
       <c r="B61" s="10">
         <v>144</v>
@@ -4549,10 +4621,14 @@
       <c r="I61" s="12">
         <v>4470</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J61" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="s">
-        <v>119</v>
+        <v>68</v>
       </c>
       <c r="B62" s="10">
         <v>36</v>
@@ -4578,10 +4654,14 @@
       <c r="I62" s="15">
         <v>5737</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J62">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="9" t="s">
-        <v>120</v>
+        <v>69</v>
       </c>
       <c r="B63" s="10">
         <v>74</v>
@@ -4607,10 +4687,14 @@
       <c r="I63" s="15">
         <v>2901</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J63" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="9" t="s">
-        <v>121</v>
+        <v>70</v>
       </c>
       <c r="B64" s="10">
         <v>0</v>
@@ -4635,6 +4719,10 @@
       </c>
       <c r="I64" s="15">
         <v>0</v>
+      </c>
+      <c r="J64" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
@@ -4689,7 +4777,7 @@
     </row>
     <row r="70" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="21" t="s">
-        <v>122</v>
+        <v>71</v>
       </c>
       <c r="B70" s="22"/>
       <c r="C70" s="22"/>
@@ -4795,7 +4883,7 @@
     </row>
     <row r="2" spans="1:14" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>123</v>
+        <v>72</v>
       </c>
       <c r="B2" s="41"/>
       <c r="C2" s="41"/>
@@ -4816,22 +4904,22 @@
         <v>14</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>124</v>
+        <v>73</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>125</v>
+        <v>74</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>126</v>
+        <v>75</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>127</v>
+        <v>76</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>128</v>
+        <v>77</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>129</v>
+        <v>78</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>21</v>
@@ -4840,16 +4928,16 @@
         <v>22</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>131</v>
+        <v>80</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>133</v>
+        <v>82</v>
       </c>
       <c r="N3" s="24"/>
     </row>
@@ -5141,7 +5229,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="21" t="s">
-        <v>134</v>
+        <v>83</v>
       </c>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
@@ -5159,7 +5247,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="19" t="s">
-        <v>135</v>
+        <v>84</v>
       </c>
       <c r="B13" s="20"/>
       <c r="C13" s="20"/>
@@ -5180,7 +5268,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="21" t="s">
-        <v>136</v>
+        <v>85</v>
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>
@@ -5283,7 +5371,7 @@
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>137</v>
+        <v>86</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -5300,7 +5388,7 @@
     </row>
     <row r="3" spans="1:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>138</v>
+        <v>87</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -5320,22 +5408,22 @@
         <v>28</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>124</v>
+        <v>73</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>125</v>
+        <v>74</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>126</v>
+        <v>75</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>127</v>
+        <v>76</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>128</v>
+        <v>77</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>129</v>
+        <v>78</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>21</v>
@@ -5344,16 +5432,16 @@
         <v>22</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>131</v>
+        <v>80</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>133</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -6548,7 +6636,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="21" t="s">
-        <v>134</v>
+        <v>83</v>
       </c>
       <c r="B43" s="22"/>
       <c r="C43" s="18"/>
@@ -6565,7 +6653,7 @@
     </row>
     <row r="44" spans="1:13" ht="14.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="19" t="s">
-        <v>135</v>
+        <v>84</v>
       </c>
       <c r="B44" s="22"/>
       <c r="C44" s="20"/>
@@ -6583,7 +6671,7 @@
     <row r="45" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="21" t="s">
-        <v>136</v>
+        <v>85</v>
       </c>
       <c r="B46" s="22"/>
       <c r="C46" s="18"/>
@@ -6638,9 +6726,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M75"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6678,7 +6766,7 @@
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>139</v>
+        <v>88</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -6698,22 +6786,22 @@
         <v>63</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>124</v>
+        <v>73</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>125</v>
+        <v>74</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>126</v>
+        <v>75</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>127</v>
+        <v>76</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>128</v>
+        <v>77</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>129</v>
+        <v>78</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>21</v>
@@ -6722,16 +6810,16 @@
         <v>22</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>131</v>
+        <v>80</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>140</v>
+        <v>89</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>133</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -6852,7 +6940,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="B8" s="10">
         <v>997828</v>
@@ -6893,7 +6981,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="B9" s="10">
         <v>95519</v>
@@ -6934,7 +7022,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="B10" s="10">
         <v>1295512</v>
@@ -6975,7 +7063,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="B11" s="10">
         <v>607318</v>
@@ -7016,7 +7104,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="B12" s="10">
         <v>5938760</v>
@@ -7057,7 +7145,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="B13" s="10">
         <v>883009</v>
@@ -7098,7 +7186,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="B14" s="10">
         <v>636811</v>
@@ -7139,7 +7227,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>73</v>
+        <v>101</v>
       </c>
       <c r="B15" s="10">
         <v>206519</v>
@@ -7180,7 +7268,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>74</v>
+        <v>102</v>
       </c>
       <c r="B16" s="10">
         <v>78998</v>
@@ -7221,7 +7309,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
       <c r="B17" s="10">
         <v>4507789</v>
@@ -7262,7 +7350,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="B18" s="10">
         <v>1679548</v>
@@ -7303,7 +7391,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="B19" s="10">
         <v>251192</v>
@@ -7344,7 +7432,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
       <c r="B20" s="10">
         <v>336675</v>
@@ -7385,7 +7473,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
       <c r="B21" s="10">
         <v>2093239</v>
@@ -7426,7 +7514,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="B22" s="10">
         <v>1211086</v>
@@ -7467,7 +7555,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="B23" s="10">
         <v>604029</v>
@@ -7508,7 +7596,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="B24" s="10">
         <v>512113</v>
@@ -7549,7 +7637,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="B25" s="10">
         <v>890924</v>
@@ -7590,7 +7678,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="B26" s="10">
         <v>832317</v>
@@ -7631,7 +7719,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>85</v>
+        <v>113</v>
       </c>
       <c r="B27" s="10">
         <v>330784</v>
@@ -7672,7 +7760,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
-        <v>86</v>
+        <v>114</v>
       </c>
       <c r="B28" s="10">
         <v>930633</v>
@@ -7713,7 +7801,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
-        <v>87</v>
+        <v>115</v>
       </c>
       <c r="B29" s="10">
         <v>1238208</v>
@@ -7754,7 +7842,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
       <c r="B30" s="10">
         <v>2000130</v>
@@ -7795,7 +7883,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="B31" s="10">
         <v>990337</v>
@@ -7836,7 +7924,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="B32" s="10">
         <v>576868</v>
@@ -7877,7 +7965,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="B33" s="10">
         <v>1171420</v>
@@ -7918,7 +8006,7 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="B34" s="10">
         <v>226106</v>
@@ -7959,7 +8047,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
       <c r="B35" s="10">
         <v>331650</v>
@@ -8000,7 +8088,7 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
-        <v>94</v>
+        <v>122</v>
       </c>
       <c r="B36" s="10">
         <v>507524</v>
@@ -8041,7 +8129,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="B37" s="10">
         <v>283716</v>
@@ -8082,7 +8170,7 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
-        <v>96</v>
+        <v>124</v>
       </c>
       <c r="B38" s="10">
         <v>1485510</v>
@@ -8123,7 +8211,7 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
       <c r="B39" s="10">
         <v>404483</v>
@@ -8164,7 +8252,7 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
-        <v>98</v>
+        <v>126</v>
       </c>
       <c r="B40" s="10">
         <v>3371357</v>
@@ -8205,7 +8293,7 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
-        <v>99</v>
+        <v>127</v>
       </c>
       <c r="B41" s="10">
         <v>1952241</v>
@@ -8246,7 +8334,7 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
-        <v>100</v>
+        <v>128</v>
       </c>
       <c r="B42" s="10">
         <v>126220</v>
@@ -8287,7 +8375,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="B43" s="10">
         <v>2238176</v>
@@ -8328,7 +8416,7 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="B44" s="10">
         <v>698229</v>
@@ -8369,7 +8457,7 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
-        <v>103</v>
+        <v>131</v>
       </c>
       <c r="B45" s="10">
         <v>832435</v>
@@ -8410,7 +8498,7 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="B46" s="10">
         <v>2579811</v>
@@ -8451,7 +8539,7 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="B47" s="10">
         <v>204871</v>
@@ -8492,7 +8580,7 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
-        <v>106</v>
+        <v>134</v>
       </c>
       <c r="B48" s="10">
         <v>1065886</v>
@@ -8533,7 +8621,7 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="9" t="s">
-        <v>107</v>
+        <v>135</v>
       </c>
       <c r="B49" s="10">
         <v>169986</v>
@@ -8574,7 +8662,7 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
-        <v>108</v>
+        <v>136</v>
       </c>
       <c r="B50" s="10">
         <v>1309473</v>
@@ -8615,7 +8703,7 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="9" t="s">
-        <v>109</v>
+        <v>137</v>
       </c>
       <c r="B51" s="10">
         <v>4014133</v>
@@ -8656,7 +8744,7 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="s">
-        <v>110</v>
+        <v>138</v>
       </c>
       <c r="B52" s="10">
         <v>389683</v>
@@ -8697,7 +8785,7 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="9" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="B53" s="10">
         <v>142369</v>
@@ -8738,7 +8826,7 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="9" t="s">
-        <v>112</v>
+        <v>140</v>
       </c>
       <c r="B54" s="10">
         <v>1423305</v>
@@ -8779,7 +8867,7 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="9" t="s">
-        <v>113</v>
+        <v>141</v>
       </c>
       <c r="B55" s="10">
         <v>1305985</v>
@@ -8820,7 +8908,7 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="9" t="s">
-        <v>114</v>
+        <v>142</v>
       </c>
       <c r="B56" s="10">
         <v>415226</v>
@@ -8861,7 +8949,7 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="9" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="B57" s="10">
         <v>1149284</v>
@@ -8902,7 +8990,7 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="9" t="s">
-        <v>116</v>
+        <v>144</v>
       </c>
       <c r="B58" s="10">
         <v>108349</v>
@@ -8960,7 +9048,7 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="17" t="s">
-        <v>117</v>
+        <v>67</v>
       </c>
       <c r="B60" s="59"/>
       <c r="C60" s="59"/>
@@ -8977,7 +9065,7 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="9" t="s">
-        <v>118</v>
+        <v>145</v>
       </c>
       <c r="B61" s="10">
         <v>657520</v>
@@ -9018,7 +9106,7 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="s">
-        <v>141</v>
+        <v>90</v>
       </c>
       <c r="B62" s="10">
         <v>36066</v>
@@ -9059,7 +9147,7 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" s="9" t="s">
-        <v>120</v>
+        <v>69</v>
       </c>
       <c r="B63" s="10">
         <v>49230</v>
@@ -9100,7 +9188,7 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="9" t="s">
-        <v>121</v>
+        <v>70</v>
       </c>
       <c r="B64" s="10">
         <v>234</v>
@@ -9190,7 +9278,7 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" s="21" t="s">
-        <v>134</v>
+        <v>83</v>
       </c>
       <c r="B69" s="22"/>
       <c r="C69" s="18"/>
@@ -9207,7 +9295,7 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" s="19" t="s">
-        <v>135</v>
+        <v>84</v>
       </c>
       <c r="B70" s="22"/>
       <c r="C70" s="20"/>
@@ -9224,7 +9312,7 @@
     </row>
     <row r="71" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="21" t="s">
-        <v>142</v>
+        <v>91</v>
       </c>
       <c r="B71" s="22"/>
       <c r="C71" s="22"/>
@@ -9242,7 +9330,7 @@
     <row r="72" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" s="21" t="s">
-        <v>136</v>
+        <v>85</v>
       </c>
       <c r="B73" s="22"/>
       <c r="C73" s="18"/>

</xml_diff>